<commit_message>
Custom avlo to increase transp motor gas use
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jshepard/Projects/state-eps-data-repository/VA/trans/AVLo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Nevada\NV_model\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF7B83D-0933-0D49-AECC-8D407C64A5D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AFEA12-372E-40FC-A804-CFA410CF4FC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="15" windowWidth="22635" windowHeight="13695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1870,10 +1870,10 @@
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="85.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2135,11 +2135,11 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.6640625" customWidth="1"/>
+    <col min="1" max="1" width="73.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="102.33203125" customWidth="1"/>
+    <col min="3" max="3" width="102.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2411,7 +2411,7 @@
         <v>33.023738872403563</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16">
+    <row r="36" spans="1:3">
       <c r="A36" s="10" t="s">
         <v>47</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>48.656731685074099</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16">
+    <row r="37" spans="1:3">
       <c r="A37" s="10" t="s">
         <v>113</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>17287</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16">
+    <row r="60" spans="1:2">
       <c r="A60" s="10" t="s">
         <v>57</v>
       </c>
@@ -2665,16 +2665,16 @@
   <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="48">
+    <row r="1" spans="1:37" ht="45">
       <c r="A1" s="19" t="s">
         <v>111</v>
       </c>
@@ -2792,147 +2792,147 @@
         <v>12</v>
       </c>
       <c r="B2" s="7">
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="C2" s="7">
         <f>$B2</f>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:AK7" si="0">$B2</f>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="F2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="I2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="P2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="Q2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="R2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="S2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="T2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="U2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="V2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="W2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="X2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="Y2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="Z2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AA2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AB2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AC2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AD2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AE2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AG2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AH2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AI2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AJ2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="AK2" s="7">
         <f t="shared" si="0"/>
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -3693,12 +3693,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="32">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="45">
       <c r="A1" s="19" t="s">
         <v>112</v>
       </c>

</xml_diff>